<commit_message>
finished control unit الحمدلله
</commit_message>
<xml_diff>
--- a/singals_instruction_values.xlsx
+++ b/singals_instruction_values.xlsx
@@ -1416,10 +1416,10 @@
   <sheetPr/>
   <dimension ref="A1:AL30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A18" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A19" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="B10" sqref="B10"/>
+      <selection pane="topRight" activeCell="Z1" sqref="Z1:AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="21"/>
@@ -2034,7 +2034,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="27" t="str">
-        <f t="shared" si="0"/>
+        <f>I6&amp;J6&amp;K6&amp;L6&amp;M6&amp;N6&amp;O6&amp;P6&amp;Q6&amp;R6&amp;S6&amp;T6&amp;U6&amp;V6&amp;W6&amp;X6&amp;Y6&amp;Z6&amp;AA6&amp;AB6&amp;AC6&amp;AD6&amp;AE6&amp;AF6&amp;AG6&amp;AH6&amp;AI6&amp;AJ6&amp;AK6&amp;AL6</f>
         <v>000001100010000000100000110000</v>
       </c>
       <c r="I6" s="7">
@@ -3177,7 +3177,7 @@
       </c>
       <c r="H17" s="27" t="str">
         <f t="shared" si="4"/>
-        <v>00000000001000000001000000100</v>
+        <v>000000000010000000001000000100</v>
       </c>
       <c r="I17" s="7">
         <v>0</v>
@@ -3233,7 +3233,9 @@
       <c r="Z17" s="7">
         <v>0</v>
       </c>
-      <c r="AA17" s="7"/>
+      <c r="AA17" s="7">
+        <v>0</v>
+      </c>
       <c r="AB17" s="7">
         <v>0</v>
       </c>
@@ -3686,7 +3688,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="27" t="str">
-        <f t="shared" ref="H22:H29" si="5">I22&amp;J22&amp;K22&amp;L22&amp;M22&amp;N22&amp;O22&amp;P22&amp;Q22&amp;R22&amp;S22&amp;T22&amp;U22&amp;V22&amp;W22&amp;X22&amp;Y22&amp;Z22&amp;AA22&amp;AB22&amp;AC22&amp;AD22&amp;AE22&amp;AF22&amp;AG22&amp;AH22&amp;AI22&amp;AJ22&amp;AK22&amp;AL22</f>
+        <f>I22&amp;J22&amp;K22&amp;L22&amp;M22&amp;N22&amp;O22&amp;P22&amp;Q22&amp;R22&amp;S22&amp;T22&amp;U22&amp;V22&amp;W22&amp;X22&amp;Y22&amp;Z22&amp;AA22&amp;AB22&amp;AC22&amp;AD22&amp;AE22&amp;AF22&amp;AG22&amp;AH22&amp;AI22&amp;AJ22&amp;AK22&amp;AL22</f>
         <v>000000000000000000000001001000</v>
       </c>
       <c r="I22" s="7">
@@ -3804,7 +3806,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="27" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="H22:H29" si="5">I23&amp;J23&amp;K23&amp;L23&amp;M23&amp;N23&amp;O23&amp;P23&amp;Q23&amp;R23&amp;S23&amp;T23&amp;U23&amp;V23&amp;W23&amp;X23&amp;Y23&amp;Z23&amp;AA23&amp;AB23&amp;AC23&amp;AD23&amp;AE23&amp;AF23&amp;AG23&amp;AH23&amp;AI23&amp;AJ23&amp;AK23&amp;AL23</f>
         <v>000000000000000000000010001000</v>
       </c>
       <c r="I23" s="7">
@@ -8633,7 +8635,7 @@
       </c>
       <c r="B17" s="1" t="str">
         <f>IF(Sheet1!H17&lt;&gt;Sheet2!B17,"Sheet1:"&amp;Sheet1!H17&amp;" vs Sheet2:"&amp;Sheet2!B17,"")</f>
-        <v>Sheet1:00000000001000000001000000100 vs Sheet2:</v>
+        <v>Sheet1:000000000010000000001000000100 vs Sheet2:</v>
       </c>
       <c r="C17" s="1" t="str">
         <f>IF(Sheet1!I17&lt;&gt;Sheet2!C17,"Sheet1:"&amp;Sheet1!I17&amp;" vs Sheet2:"&amp;Sheet2!C17,"")</f>

</xml_diff>

<commit_message>
fix typo in rst in ctrl and sheet
</commit_message>
<xml_diff>
--- a/singals_instruction_values.xlsx
+++ b/singals_instruction_values.xlsx
@@ -195,8 +195,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="26">
@@ -256,14 +256,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -271,6 +271,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,7 +293,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -299,9 +315,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -316,29 +346,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -363,14 +371,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -467,31 +467,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -503,103 +497,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -617,7 +515,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -629,7 +623,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -641,13 +647,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -739,26 +739,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -780,44 +771,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -836,12 +792,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -859,130 +859,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="40" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="40" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1550,10 +1550,10 @@
       <c r="G2" s="26"/>
       <c r="H2" s="27" t="str">
         <f>I2&amp;J2&amp;K2&amp;L2&amp;M2&amp;N2&amp;O2&amp;P2&amp;Q2&amp;R2&amp;S2&amp;T2&amp;U2&amp;V2&amp;W2&amp;X2&amp;Y2&amp;Z2&amp;AA2&amp;AB2&amp;AC2&amp;AD2&amp;AE2&amp;AF2&amp;AG2&amp;AH2&amp;AI2&amp;AJ2&amp;AK2&amp;AL2</f>
-        <v>100000000000000000000000000000</v>
+        <v>000000000000000100000000000000</v>
       </c>
       <c r="I2" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="7">
         <v>0</v>
@@ -1598,7 +1598,7 @@
         <v>0</v>
       </c>
       <c r="X2" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
assembler one + two operands
</commit_message>
<xml_diff>
--- a/singals_instruction_values.xlsx
+++ b/singals_instruction_values.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="71">
   <si>
     <t>Instruction</t>
   </si>
@@ -108,6 +108,72 @@
     <t>SETC</t>
   </si>
   <si>
+    <t>NOT Rd</t>
+  </si>
+  <si>
+    <t>INC Rd</t>
+  </si>
+  <si>
+    <t>OUT R2</t>
+  </si>
+  <si>
+    <t>IN Rd</t>
+  </si>
+  <si>
+    <t>Mov Rd, R1</t>
+  </si>
+  <si>
+    <t>Add Rd, R1, R2</t>
+  </si>
+  <si>
+    <t>SUB Rd, R1, R2</t>
+  </si>
+  <si>
+    <t>AND Rd, R1, R2</t>
+  </si>
+  <si>
+    <t>iadd, rd, r1, imm</t>
+  </si>
+  <si>
+    <t>push r2</t>
+  </si>
+  <si>
+    <t>pop rd</t>
+  </si>
+  <si>
+    <t>ldm rd, imm</t>
+  </si>
+  <si>
+    <t>ld rd, R1+offset</t>
+  </si>
+  <si>
+    <t>std r2, r1+offset</t>
+  </si>
+  <si>
+    <t>jz r</t>
+  </si>
+  <si>
+    <t>jn r</t>
+  </si>
+  <si>
+    <t>jc r</t>
+  </si>
+  <si>
+    <t>jmp r</t>
+  </si>
+  <si>
+    <t>call r</t>
+  </si>
+  <si>
+    <t>ret</t>
+  </si>
+  <si>
+    <t>INT index</t>
+  </si>
+  <si>
+    <t>ret int</t>
+  </si>
+  <si>
     <t>NOT Rdst</t>
   </si>
   <si>
@@ -150,30 +216,6 @@
     <t>std rs1, rs2+offset</t>
   </si>
   <si>
-    <t>jz r</t>
-  </si>
-  <si>
-    <t>jn r</t>
-  </si>
-  <si>
-    <t>jc r</t>
-  </si>
-  <si>
-    <t>jmp r</t>
-  </si>
-  <si>
-    <t>call r</t>
-  </si>
-  <si>
-    <t>ret</t>
-  </si>
-  <si>
-    <t>INT index</t>
-  </si>
-  <si>
-    <t>ret int</t>
-  </si>
-  <si>
     <t>0-?1</t>
   </si>
   <si>
@@ -194,10 +236,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -249,14 +291,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -277,14 +312,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -292,54 +319,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -360,6 +342,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -376,17 +397,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -467,13 +509,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,7 +527,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -503,19 +563,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -533,13 +581,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,13 +599,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -575,13 +647,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -593,61 +683,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -754,6 +796,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -769,15 +820,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -789,6 +831,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -810,15 +861,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -831,8 +873,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -841,13 +883,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -859,130 +901,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1413,10 +1455,10 @@
   <sheetPr/>
   <dimension ref="A1:AL32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A13" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="H2" sqref="H2"/>
+      <selection pane="topRight" activeCell="A18" sqref="A18:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="21"/>
@@ -5020,7 +5062,7 @@
     </row>
     <row r="5" ht="42.75" spans="1:32">
       <c r="A5" s="8" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="7"/>
@@ -5072,7 +5114,7 @@
     </row>
     <row r="6" ht="42.75" spans="1:32">
       <c r="A6" s="8" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="7"/>
@@ -5126,7 +5168,7 @@
     </row>
     <row r="7" ht="42.75" spans="1:32">
       <c r="A7" s="8" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="7"/>
@@ -5176,7 +5218,7 @@
     </row>
     <row r="8" ht="42.75" spans="1:32">
       <c r="A8" s="8" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="7"/>
@@ -5262,7 +5304,7 @@
     </row>
     <row r="10" ht="42.75" spans="1:32">
       <c r="A10" s="8" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="7"/>
@@ -5312,7 +5354,7 @@
     </row>
     <row r="11" ht="42.75" spans="1:32">
       <c r="A11" s="8" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="7"/>
@@ -5366,7 +5408,7 @@
     </row>
     <row r="12" ht="42.75" spans="1:32">
       <c r="A12" s="8" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="7"/>
@@ -5420,7 +5462,7 @@
     </row>
     <row r="13" ht="42.75" spans="1:32">
       <c r="A13" s="8" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="7"/>
@@ -5472,7 +5514,7 @@
     </row>
     <row r="14" ht="63.75" spans="1:32">
       <c r="A14" s="8" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="7"/>
@@ -5560,7 +5602,7 @@
     </row>
     <row r="16" ht="21.75" spans="1:32">
       <c r="A16" s="8" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="7"/>
@@ -5614,7 +5656,7 @@
     </row>
     <row r="17" ht="21.75" spans="1:32">
       <c r="A17" s="8" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="7"/>
@@ -5670,7 +5712,7 @@
     </row>
     <row r="18" ht="42.75" spans="1:32">
       <c r="A18" s="8" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="7"/>
@@ -5720,7 +5762,7 @@
     </row>
     <row r="19" ht="63.75" spans="1:32">
       <c r="A19" s="8" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="7"/>
@@ -5776,7 +5818,7 @@
     </row>
     <row r="20" ht="84.75" spans="1:32">
       <c r="A20" s="8" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="7"/>
@@ -5872,7 +5914,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7">
@@ -5891,7 +5933,7 @@
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
       <c r="R22" s="7" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="S22" s="7"/>
       <c r="T22" s="7">
@@ -5926,7 +5968,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7">
@@ -5945,7 +5987,7 @@
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
       <c r="R23" s="7" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="S23" s="7"/>
       <c r="T23" s="7">
@@ -5980,7 +6022,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7">
@@ -5999,7 +6041,7 @@
       <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
       <c r="R24" s="7" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="S24" s="7"/>
       <c r="T24" s="7">
@@ -6038,7 +6080,7 @@
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
@@ -6092,7 +6134,7 @@
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
@@ -6156,7 +6198,7 @@
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
@@ -6208,7 +6250,7 @@
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="12" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D28" s="7">
         <v>1</v>
@@ -6218,7 +6260,7 @@
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
@@ -6245,7 +6287,7 @@
       </c>
       <c r="U28" s="7"/>
       <c r="V28" s="7" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="W28" s="7"/>
       <c r="X28" s="7">
@@ -6259,13 +6301,13 @@
       <c r="AB28" s="7"/>
       <c r="AC28" s="7"/>
       <c r="AD28" s="12" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="AE28" s="12" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="AF28" s="12" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" ht="21.75" spans="1:32">
@@ -6284,7 +6326,7 @@
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
@@ -7024,7 +7066,7 @@
     <row r="5" ht="90" spans="1:36">
       <c r="A5" s="1" t="str">
         <f>IF(Sheet1!A7&lt;&gt;Sheet2!A5,"Sheet1:"&amp;Sheet1!A7&amp;" vs Sheet2:"&amp;Sheet2!A5,"")</f>
-        <v/>
+        <v>Sheet1:NOT Rd vs Sheet2:NOT Rdst</v>
       </c>
       <c r="B5" s="1" t="str">
         <f>IF(Sheet1!H7&lt;&gt;Sheet2!B5,"Sheet1:"&amp;Sheet1!H7&amp;" vs Sheet2:"&amp;Sheet2!B5,"")</f>
@@ -7170,7 +7212,7 @@
     <row r="6" ht="90" spans="1:36">
       <c r="A6" s="1" t="str">
         <f>IF(Sheet1!A8&lt;&gt;Sheet2!A6,"Sheet1:"&amp;Sheet1!A8&amp;" vs Sheet2:"&amp;Sheet2!A6,"")</f>
-        <v/>
+        <v>Sheet1:INC Rd vs Sheet2:INC Rdst</v>
       </c>
       <c r="B6" s="1" t="str">
         <f>IF(Sheet1!H8&lt;&gt;Sheet2!B6,"Sheet1:"&amp;Sheet1!H8&amp;" vs Sheet2:"&amp;Sheet2!B6,"")</f>
@@ -7316,7 +7358,7 @@
     <row r="7" ht="90" spans="1:36">
       <c r="A7" s="1" t="str">
         <f>IF(Sheet1!A9&lt;&gt;Sheet2!A7,"Sheet1:"&amp;Sheet1!A9&amp;" vs Sheet2:"&amp;Sheet2!A7,"")</f>
-        <v/>
+        <v>Sheet1:OUT R2 vs Sheet2:OUT Rdst</v>
       </c>
       <c r="B7" s="1" t="str">
         <f>IF(Sheet1!H9&lt;&gt;Sheet2!B7,"Sheet1:"&amp;Sheet1!H9&amp;" vs Sheet2:"&amp;Sheet2!B7,"")</f>
@@ -7462,7 +7504,7 @@
     <row r="8" ht="90" spans="1:36">
       <c r="A8" s="1" t="str">
         <f>IF(Sheet1!A10&lt;&gt;Sheet2!A8,"Sheet1:"&amp;Sheet1!A10&amp;" vs Sheet2:"&amp;Sheet2!A8,"")</f>
-        <v/>
+        <v>Sheet1:IN Rd vs Sheet2:IN Rdst</v>
       </c>
       <c r="B8" s="1" t="str">
         <f>IF(Sheet1!H10&lt;&gt;Sheet2!B8,"Sheet1:"&amp;Sheet1!H10&amp;" vs Sheet2:"&amp;Sheet2!B8,"")</f>
@@ -7754,7 +7796,7 @@
     <row r="10" ht="90" spans="1:36">
       <c r="A10" s="1" t="str">
         <f>IF(Sheet1!A12&lt;&gt;Sheet2!A10,"Sheet1:"&amp;Sheet1!A12&amp;" vs Sheet2:"&amp;Sheet2!A10,"")</f>
-        <v/>
+        <v>Sheet1:Mov Rd, R1 vs Sheet2:Mov R, R</v>
       </c>
       <c r="B10" s="1" t="str">
         <f>IF(Sheet1!H12&lt;&gt;Sheet2!B10,"Sheet1:"&amp;Sheet1!H12&amp;" vs Sheet2:"&amp;Sheet2!B10,"")</f>
@@ -7900,7 +7942,7 @@
     <row r="11" ht="90" spans="1:36">
       <c r="A11" s="1" t="str">
         <f>IF(Sheet1!A13&lt;&gt;Sheet2!A11,"Sheet1:"&amp;Sheet1!A13&amp;" vs Sheet2:"&amp;Sheet2!A11,"")</f>
-        <v/>
+        <v>Sheet1:Add Rd, R1, R2 vs Sheet2:Add R, R, R</v>
       </c>
       <c r="B11" s="1" t="str">
         <f>IF(Sheet1!H13&lt;&gt;Sheet2!B11,"Sheet1:"&amp;Sheet1!H13&amp;" vs Sheet2:"&amp;Sheet2!B11,"")</f>
@@ -8046,7 +8088,7 @@
     <row r="12" ht="90" spans="1:36">
       <c r="A12" s="1" t="str">
         <f>IF(Sheet1!A14&lt;&gt;Sheet2!A12,"Sheet1:"&amp;Sheet1!A14&amp;" vs Sheet2:"&amp;Sheet2!A12,"")</f>
-        <v/>
+        <v>Sheet1:SUB Rd, R1, R2 vs Sheet2:SUB R, R, R</v>
       </c>
       <c r="B12" s="1" t="str">
         <f>IF(Sheet1!H14&lt;&gt;Sheet2!B12,"Sheet1:"&amp;Sheet1!H14&amp;" vs Sheet2:"&amp;Sheet2!B12,"")</f>
@@ -8192,7 +8234,7 @@
     <row r="13" ht="90" spans="1:36">
       <c r="A13" s="1" t="str">
         <f>IF(Sheet1!A15&lt;&gt;Sheet2!A13,"Sheet1:"&amp;Sheet1!A15&amp;" vs Sheet2:"&amp;Sheet2!A13,"")</f>
-        <v/>
+        <v>Sheet1:AND Rd, R1, R2 vs Sheet2:AND R, R, R</v>
       </c>
       <c r="B13" s="1" t="str">
         <f>IF(Sheet1!H15&lt;&gt;Sheet2!B13,"Sheet1:"&amp;Sheet1!H15&amp;" vs Sheet2:"&amp;Sheet2!B13,"")</f>
@@ -8338,7 +8380,7 @@
     <row r="14" ht="90" spans="1:36">
       <c r="A14" s="1" t="str">
         <f>IF(Sheet1!A16&lt;&gt;Sheet2!A14,"Sheet1:"&amp;Sheet1!A16&amp;" vs Sheet2:"&amp;Sheet2!A14,"")</f>
-        <v/>
+        <v>Sheet1:iadd, rd, r1, imm vs Sheet2:iadd, r, r, imm</v>
       </c>
       <c r="B14" s="1" t="str">
         <f>IF(Sheet1!H16&lt;&gt;Sheet2!B14,"Sheet1:"&amp;Sheet1!H16&amp;" vs Sheet2:"&amp;Sheet2!B14,"")</f>
@@ -8630,7 +8672,7 @@
     <row r="16" ht="90" spans="1:36">
       <c r="A16" s="1" t="str">
         <f>IF(Sheet1!A18&lt;&gt;Sheet2!A16,"Sheet1:"&amp;Sheet1!A18&amp;" vs Sheet2:"&amp;Sheet2!A16,"")</f>
-        <v/>
+        <v>Sheet1:push r2 vs Sheet2:push r</v>
       </c>
       <c r="B16" s="1" t="str">
         <f>IF(Sheet1!H18&lt;&gt;Sheet2!B16,"Sheet1:"&amp;Sheet1!H18&amp;" vs Sheet2:"&amp;Sheet2!B16,"")</f>
@@ -8776,7 +8818,7 @@
     <row r="17" ht="90" spans="1:36">
       <c r="A17" s="1" t="str">
         <f>IF(Sheet1!A19&lt;&gt;Sheet2!A17,"Sheet1:"&amp;Sheet1!A19&amp;" vs Sheet2:"&amp;Sheet2!A17,"")</f>
-        <v/>
+        <v>Sheet1:pop rd vs Sheet2:pop r</v>
       </c>
       <c r="B17" s="1" t="str">
         <f>IF(Sheet1!H19&lt;&gt;Sheet2!B17,"Sheet1:"&amp;Sheet1!H19&amp;" vs Sheet2:"&amp;Sheet2!B17,"")</f>
@@ -8922,7 +8964,7 @@
     <row r="18" ht="90" spans="1:36">
       <c r="A18" s="1" t="str">
         <f>IF(Sheet1!A20&lt;&gt;Sheet2!A18,"Sheet1:"&amp;Sheet1!A20&amp;" vs Sheet2:"&amp;Sheet2!A18,"")</f>
-        <v/>
+        <v>Sheet1:ldm rd, imm vs Sheet2:ldm r, imm</v>
       </c>
       <c r="B18" s="1" t="str">
         <f>IF(Sheet1!H20&lt;&gt;Sheet2!B18,"Sheet1:"&amp;Sheet1!H20&amp;" vs Sheet2:"&amp;Sheet2!B18,"")</f>
@@ -9068,7 +9110,7 @@
     <row r="19" ht="90" spans="1:36">
       <c r="A19" s="1" t="str">
         <f>IF(Sheet1!A21&lt;&gt;Sheet2!A19,"Sheet1:"&amp;Sheet1!A21&amp;" vs Sheet2:"&amp;Sheet2!A19,"")</f>
-        <v/>
+        <v>Sheet1:ld rd, R1+offset vs Sheet2:ld r, R+offset</v>
       </c>
       <c r="B19" s="1" t="str">
         <f>IF(Sheet1!H21&lt;&gt;Sheet2!B19,"Sheet1:"&amp;Sheet1!H21&amp;" vs Sheet2:"&amp;Sheet2!B19,"")</f>
@@ -9214,7 +9256,7 @@
     <row r="20" ht="90" spans="1:36">
       <c r="A20" s="1" t="str">
         <f>IF(Sheet1!A22&lt;&gt;Sheet2!A20,"Sheet1:"&amp;Sheet1!A22&amp;" vs Sheet2:"&amp;Sheet2!A20,"")</f>
-        <v/>
+        <v>Sheet1:std r2, r1+offset vs Sheet2:std rs1, rs2+offset</v>
       </c>
       <c r="B20" s="1" t="str">
         <f>IF(Sheet1!H22&lt;&gt;Sheet2!B20,"Sheet1:"&amp;Sheet1!H22&amp;" vs Sheet2:"&amp;Sheet2!B20,"")</f>

</xml_diff>

<commit_message>
ONE + TWO OPERANDS TEST CASES PASSgit add fetch.vhd  fetch_decode_buffer.vhd guidelines.txt integration.vhd memory.vhd singals_instruction_values.xlsx
</commit_message>
<xml_diff>
--- a/singals_instruction_values.xlsx
+++ b/singals_instruction_values.xlsx
@@ -1455,10 +1455,10 @@
   <sheetPr/>
   <dimension ref="A1:AL32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A13" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" topLeftCell="A18" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="A18" sqref="A18:B22"/>
+      <selection pane="topRight" activeCell="AI29" sqref="AI29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="21"/>
@@ -2104,7 +2104,7 @@
       </c>
       <c r="H7" s="27" t="str">
         <f t="shared" si="0"/>
-        <v>000001000010000000100000000000</v>
+        <v>000001000010000000100000001000</v>
       </c>
       <c r="I7" s="7">
         <v>0</v>
@@ -2185,7 +2185,7 @@
         <v>0</v>
       </c>
       <c r="AI7" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ7" s="7">
         <v>0</v>
@@ -2616,7 +2616,7 @@
       </c>
       <c r="H12" s="27" t="str">
         <f t="shared" ref="H12:H16" si="3">I12&amp;J12&amp;K12&amp;L12&amp;M12&amp;N12&amp;O12&amp;P12&amp;Q12&amp;R12&amp;S12&amp;T12&amp;U12&amp;V12&amp;W12&amp;X12&amp;Y12&amp;Z12&amp;AA12&amp;AB12&amp;AC12&amp;AD12&amp;AE12&amp;AF12&amp;AG12&amp;AH12&amp;AI12&amp;AJ12&amp;AK12&amp;AL12</f>
-        <v>000000000010000000100000001000</v>
+        <v>000000000010000000100000000000</v>
       </c>
       <c r="I12" s="7">
         <v>0</v>
@@ -2697,7 +2697,7 @@
         <v>0</v>
       </c>
       <c r="AI12" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ12" s="7">
         <v>0</v>
@@ -3246,7 +3246,7 @@
       </c>
       <c r="H18" s="27" t="str">
         <f t="shared" ref="H18:H22" si="4">I18&amp;J18&amp;K18&amp;L18&amp;M18&amp;N18&amp;O18&amp;P18&amp;Q18&amp;R18&amp;S18&amp;T18&amp;U18&amp;V18&amp;W18&amp;X18&amp;Y18&amp;Z18&amp;AA18&amp;AB18&amp;AC18&amp;AD18&amp;AE18&amp;AF18&amp;AG18&amp;AH18&amp;AI18&amp;AJ18&amp;AK18&amp;AL18</f>
-        <v>000000000000000000001000001110</v>
+        <v>000000000000000000001000000110</v>
       </c>
       <c r="I18" s="7">
         <v>0</v>
@@ -3327,7 +3327,7 @@
         <v>0</v>
       </c>
       <c r="AI18" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ18" s="7">
         <v>1</v>
@@ -3876,7 +3876,7 @@
       </c>
       <c r="H24" s="27" t="str">
         <f>I24&amp;J24&amp;K24&amp;L24&amp;M24&amp;N24&amp;O24&amp;P24&amp;Q24&amp;R24&amp;S24&amp;T24&amp;U24&amp;V24&amp;W24&amp;X24&amp;Y24&amp;Z24&amp;AA24&amp;AB24&amp;AC24&amp;AD24&amp;AE24&amp;AF24&amp;AG24&amp;AH24&amp;AI24&amp;AJ24&amp;AK24&amp;AL24</f>
-        <v>000000000000000000000001001000</v>
+        <v>000000000000000000000001000000</v>
       </c>
       <c r="I24" s="7">
         <v>0</v>
@@ -3957,7 +3957,7 @@
         <v>0</v>
       </c>
       <c r="AI24" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ24" s="7">
         <v>0</v>
@@ -3994,7 +3994,7 @@
       </c>
       <c r="H25" s="27" t="str">
         <f t="shared" ref="H24:H31" si="5">I25&amp;J25&amp;K25&amp;L25&amp;M25&amp;N25&amp;O25&amp;P25&amp;Q25&amp;R25&amp;S25&amp;T25&amp;U25&amp;V25&amp;W25&amp;X25&amp;Y25&amp;Z25&amp;AA25&amp;AB25&amp;AC25&amp;AD25&amp;AE25&amp;AF25&amp;AG25&amp;AH25&amp;AI25&amp;AJ25&amp;AK25&amp;AL25</f>
-        <v>000000000000000000000010001000</v>
+        <v>000000000000000000000010000000</v>
       </c>
       <c r="I25" s="7">
         <v>0</v>
@@ -4075,7 +4075,7 @@
         <v>0</v>
       </c>
       <c r="AI25" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ25" s="7">
         <v>0</v>
@@ -4112,7 +4112,7 @@
       </c>
       <c r="H26" s="27" t="str">
         <f t="shared" si="5"/>
-        <v>000000000000000000000011001000</v>
+        <v>000000000000000000000011000000</v>
       </c>
       <c r="I26" s="7">
         <v>0</v>
@@ -4193,7 +4193,7 @@
         <v>0</v>
       </c>
       <c r="AI26" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ26" s="7">
         <v>0</v>
@@ -4230,7 +4230,7 @@
       </c>
       <c r="H27" s="27" t="str">
         <f t="shared" si="5"/>
-        <v>011000000000000010000100001000</v>
+        <v>011000000000000010000100000000</v>
       </c>
       <c r="I27" s="7">
         <v>0</v>
@@ -4311,7 +4311,7 @@
         <v>0</v>
       </c>
       <c r="AI27" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ27" s="7">
         <v>0</v>
@@ -4348,7 +4348,7 @@
       </c>
       <c r="H28" s="27" t="str">
         <f t="shared" si="5"/>
-        <v>011000000001000010001100001111</v>
+        <v>011000000001000010001100000111</v>
       </c>
       <c r="I28" s="7">
         <v>0</v>
@@ -4429,7 +4429,7 @@
         <v>0</v>
       </c>
       <c r="AI28" s="7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ28" s="7">
         <v>1</v>
@@ -7070,7 +7070,7 @@
       </c>
       <c r="B5" s="1" t="str">
         <f>IF(Sheet1!H7&lt;&gt;Sheet2!B5,"Sheet1:"&amp;Sheet1!H7&amp;" vs Sheet2:"&amp;Sheet2!B5,"")</f>
-        <v>Sheet1:000001000010000000100000000000 vs Sheet2:</v>
+        <v>Sheet1:000001000010000000100000001000 vs Sheet2:</v>
       </c>
       <c r="C5" s="1" t="str">
         <f>IF(Sheet1!I7&lt;&gt;Sheet2!C5,"Sheet1:"&amp;Sheet1!I7&amp;" vs Sheet2:"&amp;Sheet2!C5,"")</f>
@@ -7178,7 +7178,7 @@
       </c>
       <c r="AC5" s="1" t="str">
         <f>IF(Sheet1!AI7&lt;&gt;Sheet2!AC5,"Sheet1:"&amp;Sheet1!AI7&amp;" vs Sheet2:"&amp;Sheet2!AC5,"")</f>
-        <v/>
+        <v>Sheet1:1 vs Sheet2:</v>
       </c>
       <c r="AD5" s="1" t="str">
         <f>IF(Sheet1!AJ7&lt;&gt;Sheet2!AD5,"Sheet1:"&amp;Sheet1!AJ7&amp;" vs Sheet2:"&amp;Sheet2!AD5,"")</f>
@@ -7800,7 +7800,7 @@
       </c>
       <c r="B10" s="1" t="str">
         <f>IF(Sheet1!H12&lt;&gt;Sheet2!B10,"Sheet1:"&amp;Sheet1!H12&amp;" vs Sheet2:"&amp;Sheet2!B10,"")</f>
-        <v>Sheet1:000000000010000000100000001000 vs Sheet2:</v>
+        <v>Sheet1:000000000010000000100000000000 vs Sheet2:</v>
       </c>
       <c r="C10" s="1" t="str">
         <f>IF(Sheet1!I12&lt;&gt;Sheet2!C10,"Sheet1:"&amp;Sheet1!I12&amp;" vs Sheet2:"&amp;Sheet2!C10,"")</f>
@@ -7908,7 +7908,7 @@
       </c>
       <c r="AC10" s="1" t="str">
         <f>IF(Sheet1!AI12&lt;&gt;Sheet2!AC10,"Sheet1:"&amp;Sheet1!AI12&amp;" vs Sheet2:"&amp;Sheet2!AC10,"")</f>
-        <v>Sheet1:1 vs Sheet2:</v>
+        <v/>
       </c>
       <c r="AD10" s="1" t="str">
         <f>IF(Sheet1!AJ12&lt;&gt;Sheet2!AD10,"Sheet1:"&amp;Sheet1!AJ12&amp;" vs Sheet2:"&amp;Sheet2!AD10,"")</f>
@@ -8676,7 +8676,7 @@
       </c>
       <c r="B16" s="1" t="str">
         <f>IF(Sheet1!H18&lt;&gt;Sheet2!B16,"Sheet1:"&amp;Sheet1!H18&amp;" vs Sheet2:"&amp;Sheet2!B16,"")</f>
-        <v>Sheet1:000000000000000000001000001110 vs Sheet2:</v>
+        <v>Sheet1:000000000000000000001000000110 vs Sheet2:</v>
       </c>
       <c r="C16" s="1" t="str">
         <f>IF(Sheet1!I18&lt;&gt;Sheet2!C16,"Sheet1:"&amp;Sheet1!I18&amp;" vs Sheet2:"&amp;Sheet2!C16,"")</f>
@@ -8784,7 +8784,7 @@
       </c>
       <c r="AC16" s="1" t="str">
         <f>IF(Sheet1!AI18&lt;&gt;Sheet2!AC16,"Sheet1:"&amp;Sheet1!AI18&amp;" vs Sheet2:"&amp;Sheet2!AC16,"")</f>
-        <v>Sheet1:1 vs Sheet2:</v>
+        <v/>
       </c>
       <c r="AD16" s="1" t="str">
         <f>IF(Sheet1!AJ18&lt;&gt;Sheet2!AD16,"Sheet1:"&amp;Sheet1!AJ18&amp;" vs Sheet2:"&amp;Sheet2!AD16,"")</f>
@@ -9552,7 +9552,7 @@
       </c>
       <c r="B22" s="1" t="str">
         <f>IF(Sheet1!H24&lt;&gt;Sheet2!B22,"Sheet1:"&amp;Sheet1!H24&amp;" vs Sheet2:"&amp;Sheet2!B22,"")</f>
-        <v>Sheet1:000000000000000000000001001000 vs Sheet2:</v>
+        <v>Sheet1:000000000000000000000001000000 vs Sheet2:</v>
       </c>
       <c r="C22" s="1" t="str">
         <f>IF(Sheet1!I24&lt;&gt;Sheet2!C22,"Sheet1:"&amp;Sheet1!I24&amp;" vs Sheet2:"&amp;Sheet2!C22,"")</f>
@@ -9660,7 +9660,7 @@
       </c>
       <c r="AC22" s="1" t="str">
         <f>IF(Sheet1!AI24&lt;&gt;Sheet2!AC22,"Sheet1:"&amp;Sheet1!AI24&amp;" vs Sheet2:"&amp;Sheet2!AC22,"")</f>
-        <v>Sheet1:1 vs Sheet2:</v>
+        <v/>
       </c>
       <c r="AD22" s="1" t="str">
         <f>IF(Sheet1!AJ24&lt;&gt;Sheet2!AD22,"Sheet1:"&amp;Sheet1!AJ24&amp;" vs Sheet2:"&amp;Sheet2!AD22,"")</f>
@@ -9698,7 +9698,7 @@
       </c>
       <c r="B23" s="1" t="str">
         <f>IF(Sheet1!H25&lt;&gt;Sheet2!B23,"Sheet1:"&amp;Sheet1!H25&amp;" vs Sheet2:"&amp;Sheet2!B23,"")</f>
-        <v>Sheet1:000000000000000000000010001000 vs Sheet2:</v>
+        <v>Sheet1:000000000000000000000010000000 vs Sheet2:</v>
       </c>
       <c r="C23" s="1" t="str">
         <f>IF(Sheet1!I25&lt;&gt;Sheet2!C23,"Sheet1:"&amp;Sheet1!I25&amp;" vs Sheet2:"&amp;Sheet2!C23,"")</f>
@@ -9806,7 +9806,7 @@
       </c>
       <c r="AC23" s="1" t="str">
         <f>IF(Sheet1!AI25&lt;&gt;Sheet2!AC23,"Sheet1:"&amp;Sheet1!AI25&amp;" vs Sheet2:"&amp;Sheet2!AC23,"")</f>
-        <v>Sheet1:1 vs Sheet2:</v>
+        <v/>
       </c>
       <c r="AD23" s="1" t="str">
         <f>IF(Sheet1!AJ25&lt;&gt;Sheet2!AD23,"Sheet1:"&amp;Sheet1!AJ25&amp;" vs Sheet2:"&amp;Sheet2!AD23,"")</f>
@@ -9844,7 +9844,7 @@
       </c>
       <c r="B24" s="1" t="str">
         <f>IF(Sheet1!H26&lt;&gt;Sheet2!B24,"Sheet1:"&amp;Sheet1!H26&amp;" vs Sheet2:"&amp;Sheet2!B24,"")</f>
-        <v>Sheet1:000000000000000000000011001000 vs Sheet2:</v>
+        <v>Sheet1:000000000000000000000011000000 vs Sheet2:</v>
       </c>
       <c r="C24" s="1" t="str">
         <f>IF(Sheet1!I26&lt;&gt;Sheet2!C24,"Sheet1:"&amp;Sheet1!I26&amp;" vs Sheet2:"&amp;Sheet2!C24,"")</f>
@@ -9952,7 +9952,7 @@
       </c>
       <c r="AC24" s="1" t="str">
         <f>IF(Sheet1!AI26&lt;&gt;Sheet2!AC24,"Sheet1:"&amp;Sheet1!AI26&amp;" vs Sheet2:"&amp;Sheet2!AC24,"")</f>
-        <v>Sheet1:1 vs Sheet2:</v>
+        <v/>
       </c>
       <c r="AD24" s="1" t="str">
         <f>IF(Sheet1!AJ26&lt;&gt;Sheet2!AD24,"Sheet1:"&amp;Sheet1!AJ26&amp;" vs Sheet2:"&amp;Sheet2!AD24,"")</f>
@@ -9990,7 +9990,7 @@
       </c>
       <c r="B25" s="1" t="str">
         <f>IF(Sheet1!H27&lt;&gt;Sheet2!B25,"Sheet1:"&amp;Sheet1!H27&amp;" vs Sheet2:"&amp;Sheet2!B25,"")</f>
-        <v>Sheet1:011000000000000010000100001000 vs Sheet2:</v>
+        <v>Sheet1:011000000000000010000100000000 vs Sheet2:</v>
       </c>
       <c r="C25" s="1" t="str">
         <f>IF(Sheet1!I27&lt;&gt;Sheet2!C25,"Sheet1:"&amp;Sheet1!I27&amp;" vs Sheet2:"&amp;Sheet2!C25,"")</f>
@@ -10098,7 +10098,7 @@
       </c>
       <c r="AC25" s="1" t="str">
         <f>IF(Sheet1!AI27&lt;&gt;Sheet2!AC25,"Sheet1:"&amp;Sheet1!AI27&amp;" vs Sheet2:"&amp;Sheet2!AC25,"")</f>
-        <v>Sheet1:1 vs Sheet2:</v>
+        <v/>
       </c>
       <c r="AD25" s="1" t="str">
         <f>IF(Sheet1!AJ27&lt;&gt;Sheet2!AD25,"Sheet1:"&amp;Sheet1!AJ27&amp;" vs Sheet2:"&amp;Sheet2!AD25,"")</f>
@@ -10136,7 +10136,7 @@
       </c>
       <c r="B26" s="1" t="str">
         <f>IF(Sheet1!H28&lt;&gt;Sheet2!B26,"Sheet1:"&amp;Sheet1!H28&amp;" vs Sheet2:"&amp;Sheet2!B26,"")</f>
-        <v>Sheet1:011000000001000010001100001111 vs Sheet2:</v>
+        <v>Sheet1:011000000001000010001100000111 vs Sheet2:</v>
       </c>
       <c r="C26" s="1" t="str">
         <f>IF(Sheet1!I28&lt;&gt;Sheet2!C26,"Sheet1:"&amp;Sheet1!I28&amp;" vs Sheet2:"&amp;Sheet2!C26,"")</f>
@@ -10244,7 +10244,7 @@
       </c>
       <c r="AC26" s="1" t="str">
         <f>IF(Sheet1!AI28&lt;&gt;Sheet2!AC26,"Sheet1:"&amp;Sheet1!AI28&amp;" vs Sheet2:"&amp;Sheet2!AC26,"")</f>
-        <v>Sheet1:1 vs Sheet2:</v>
+        <v/>
       </c>
       <c r="AD26" s="1" t="str">
         <f>IF(Sheet1!AJ28&lt;&gt;Sheet2!AD26,"Sheet1:"&amp;Sheet1!AJ28&amp;" vs Sheet2:"&amp;Sheet2!AD26,"")</f>

</xml_diff>